<commit_message>
Update template export list of document
</commit_message>
<xml_diff>
--- a/src/main/resources/static/templates/excel/Template_E_Document.xlsx
+++ b/src/main/resources/static/templates/excel/Template_E_Document.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\FW_DMS\src\main\resources\static\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC80B9C-B7A5-45D1-A2F6-2FB8079C88F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC553AC6-5EDB-4BF2-9710-E4BBA3A094F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>STT</t>
   </si>
@@ -33,34 +33,40 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>List of documents</t>
-  </si>
-  <si>
-    <t>Rights</t>
-  </si>
-  <si>
-    <t>Read</t>
-  </si>
-  <si>
-    <t>Update</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>Share</t>
-  </si>
-  <si>
-    <t>Move</t>
-  </si>
-  <si>
-    <t>Upload at</t>
-  </si>
-  <si>
-    <t>Upload by</t>
+    <t>Người tạo</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Vị trí</t>
+  </si>
+  <si>
+    <t>Danh sách tài liệu</t>
+  </si>
+  <si>
+    <t>Phân quyền sử dụng</t>
+  </si>
+  <si>
+    <t>Quyền xem</t>
+  </si>
+  <si>
+    <t>Quyền chỉnh sửa</t>
+  </si>
+  <si>
+    <t>Quyền xóa</t>
+  </si>
+  <si>
+    <t>Quyền di chuyển</t>
+  </si>
+  <si>
+    <t>Quyền chia sẽ</t>
+  </si>
+  <si>
+    <t>Thông tin chung</t>
+  </si>
+  <si>
+    <t>Loại</t>
   </si>
 </sst>
 </file>
@@ -92,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,64 +121,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -455,99 +414,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="11" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
+      <c r="A1" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="5"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="3">
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>